<commit_message>
added all the analysis files
</commit_message>
<xml_diff>
--- a/data/codebooks/diabetes_features_by_year.xlsx
+++ b/data/codebooks/diabetes_features_by_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ML\DU\repos\projects\project-2\DU-project-2\data\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F01708F-7026-4ECF-A335-BACA9B2F14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799416B9-307E-419D-A821-FC33FDF9BE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="5570" windowWidth="19930" windowHeight="14890" xr2:uid="{B2F01B8D-487D-4741-B5A2-CECB8B1A02EE}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="19958" windowHeight="13680" xr2:uid="{B2F01B8D-487D-4741-B5A2-CECB8B1A02EE}"/>
   </bookViews>
   <sheets>
     <sheet name="diabetes_features_by_year" sheetId="1" r:id="rId1"/>
@@ -342,7 +342,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +490,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +677,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -832,19 +844,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -890,15 +905,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1242,7 +1249,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W20" sqref="W20"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,7 +1423,7 @@
       <c r="V2" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="6" t="s">
         <v>52</v>
       </c>
       <c r="X2" t="s">
@@ -1520,7 +1527,7 @@
       <c r="V3" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="6" t="s">
         <v>55</v>
       </c>
       <c r="X3" t="s">
@@ -1624,7 +1631,7 @@
       <c r="V4" t="s">
         <v>1</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="8" t="s">
         <v>80</v>
       </c>
       <c r="X4" t="s">
@@ -1665,7 +1672,7 @@
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1736,7 +1743,7 @@
       <c r="V6" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="W6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="X6" t="s">
@@ -1840,7 +1847,7 @@
       <c r="V7" t="s">
         <v>1</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="4" t="s">
         <v>78</v>
       </c>
       <c r="X7" t="s">
@@ -1944,7 +1951,7 @@
       <c r="V8" t="s">
         <v>2</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="W8" s="5" t="s">
         <v>46</v>
       </c>
       <c r="X8" t="s">
@@ -1985,7 +1992,7 @@
       <c r="A9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="W9" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2056,7 +2063,7 @@
       <c r="V10" t="s">
         <v>2</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="W10" t="s">
         <v>11</v>
       </c>
       <c r="X10" t="s">
@@ -2160,7 +2167,7 @@
       <c r="V11" t="s">
         <v>1</v>
       </c>
-      <c r="W11" s="6" t="s">
+      <c r="W11" s="5" t="s">
         <v>77</v>
       </c>
       <c r="X11" t="s">
@@ -2368,7 +2375,7 @@
       <c r="V13" t="s">
         <v>2</v>
       </c>
-      <c r="W13" s="4" t="s">
+      <c r="W13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X13" t="s">
@@ -2472,7 +2479,7 @@
       <c r="V14" t="s">
         <v>2</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="X14" t="s">
@@ -2576,7 +2583,7 @@
       <c r="V15" t="s">
         <v>1</v>
       </c>
-      <c r="W15" s="6" t="s">
+      <c r="W15" s="5" t="s">
         <v>95</v>
       </c>
       <c r="X15" t="s">
@@ -2680,7 +2687,7 @@
       <c r="V16" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="6" t="s">
+      <c r="W16" s="4" t="s">
         <v>98</v>
       </c>
       <c r="X16" t="s">
@@ -2784,7 +2791,7 @@
       <c r="V17" t="s">
         <v>2</v>
       </c>
-      <c r="W17" s="4" t="s">
+      <c r="W17" t="s">
         <v>3</v>
       </c>
       <c r="X17" t="s">
@@ -2888,7 +2895,7 @@
       <c r="V18" t="s">
         <v>1</v>
       </c>
-      <c r="W18" s="4" t="s">
+      <c r="W18" t="s">
         <v>97</v>
       </c>
       <c r="X18" t="s">
@@ -2992,7 +2999,7 @@
       <c r="V19" t="s">
         <v>2</v>
       </c>
-      <c r="W19" s="6" t="s">
+      <c r="W19" s="4" t="s">
         <v>81</v>
       </c>
       <c r="X19" t="s">
@@ -3096,7 +3103,7 @@
       <c r="V20" t="s">
         <v>1</v>
       </c>
-      <c r="W20" s="6" t="s">
+      <c r="W20" s="4" t="s">
         <v>79</v>
       </c>
       <c r="X20" t="s">
@@ -8545,7 +8552,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:AH8 A9:V9 X9:AH9 A10:AH11 A12:V12 X12:AH12 A13:AH18 A19:V19 X19:AH19 A20:AH20 A21:V21 X21:AH21 A22:AH23 A24:V24 X24:AH24 A25:AH29 A30:V30 X30:AH30 A31:AH40 A41:V41 X41:AH41 A42:AH43 A44:V44 X44:AH44 A45:AH54 A55:V55 X55:AH55 A56:AH68 A69:V69 X69:AH69 A70:AH71">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>